<commit_message>
set.ambiguous.to is NA by default
</commit_message>
<xml_diff>
--- a/Reservoir_Layer/Data/Mastomys_natalensis_presences.xlsx
+++ b/Reservoir_Layer/Data/Mastomys_natalensis_presences.xlsx
@@ -5,41 +5,42 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="M. natalensis" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Raw_M_natalensis_presences" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Cleaned_M_natalensis_presences" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'M. natalensis'!$A$1:$J$695</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Raw_M_natalensis_presences!$A$1:$J$695</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">summary!$A$1:$C$37</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_64771776_FB6F_11DE_9C8D_000D93C12944_.wvu.PrintArea" vbProcedure="false">summary!$A$1:$C$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="Z_64771776_FB6F_11DE_9C8D_000D93C12944_.wvu.PrintArea" vbProcedure="false">'M. natalensis'!$A$1:$J$695</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="Z_64771776_FB6F_11DE_9C8D_000D93C12944_.wvu.PrintTitles" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'M. natalensis'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="Z_64771776_FB6F_11DE_9C8D_000D93C12944_.wvu.PrintArea" vbProcedure="false">Raw_M_natalensis_presences!$A$1:$J$695</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="Z_64771776_FB6F_11DE_9C8D_000D93C12944_.wvu.PrintTitles" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Raw_M_natalensis_presences!$1:$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -7722,7 +7723,7 @@
   </sheetPr>
   <dimension ref="A1:V1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D718" activeCellId="0" sqref="D718"/>
     </sheetView>
   </sheetViews>
@@ -28329,7 +28330,7 @@
   </sheetPr>
   <dimension ref="A1:L168"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>

</xml_diff>